<commit_message>
#143 add exposure metrics
</commit_message>
<xml_diff>
--- a/metadata/pk_spec.xlsx
+++ b/metadata/pk_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff.dickinson\Documents\GitHub\examples\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F740EE8-210D-40A4-8735-52E2CA73AFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0C8541-8641-426F-8D37-58C16A89F5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Documents!$A$1:$C$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Methods!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$235</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$P$237</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">WhereClauses!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="576">
   <si>
     <t>Attribute</t>
   </si>
@@ -1777,6 +1777,18 @@
   </si>
   <si>
     <t>STUDYID, USUBJID</t>
+  </si>
+  <si>
+    <t>AUCSS</t>
+  </si>
+  <si>
+    <t>Steady-State AUC (ug*h/mL)</t>
+  </si>
+  <si>
+    <t>CMAXSS</t>
+  </si>
+  <si>
+    <t>Steady-State Cmax (ug/mL)</t>
   </si>
 </sst>
 </file>
@@ -2589,13 +2601,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P257"/>
+  <dimension ref="A1:P259"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D202" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D229" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N216" sqref="N216"/>
+      <selection pane="bottomRight" activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7004,7 +7016,7 @@
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A191" s="27">
+      <c r="A191">
         <v>1</v>
       </c>
       <c r="B191" s="15" t="s">
@@ -7027,7 +7039,7 @@
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" s="27">
+      <c r="A192">
         <v>2</v>
       </c>
       <c r="B192" s="15" t="s">
@@ -7052,8 +7064,8 @@
         <v>402</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A193" s="27">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193">
         <v>3</v>
       </c>
       <c r="B193" s="15" t="s">
@@ -7075,8 +7087,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A194" s="27">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194">
         <v>4</v>
       </c>
       <c r="B194" s="15" t="s">
@@ -7098,8 +7110,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A195" s="27">
+    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195">
         <v>5</v>
       </c>
       <c r="B195" s="15" t="s">
@@ -7121,8 +7133,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="27">
+    <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196">
         <v>6</v>
       </c>
       <c r="B196" s="15" t="s">
@@ -7144,8 +7156,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A197" s="27">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197">
         <v>7</v>
       </c>
       <c r="B197" s="15" t="s">
@@ -7167,8 +7179,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A198" s="27">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198">
         <v>8</v>
       </c>
       <c r="B198" s="15" t="s">
@@ -7190,8 +7202,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A199" s="27">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199">
         <v>9</v>
       </c>
       <c r="B199" s="15" t="s">
@@ -7213,8 +7225,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A200" s="27">
+    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200">
         <v>10</v>
       </c>
       <c r="B200" s="15" t="s">
@@ -7236,8 +7248,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A201" s="27">
+    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201">
         <v>11</v>
       </c>
       <c r="B201" s="15" t="s">
@@ -7259,8 +7271,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A202" s="27">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202">
         <v>12</v>
       </c>
       <c r="B202" s="15" t="s">
@@ -7282,8 +7294,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A203" s="27">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203">
         <v>13</v>
       </c>
       <c r="B203" s="15" t="s">
@@ -7305,8 +7317,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="27">
+    <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A204">
         <v>14</v>
       </c>
       <c r="B204" s="15" t="s">
@@ -7328,8 +7340,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A205" s="27">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205">
         <v>15</v>
       </c>
       <c r="B205" s="15" t="s">
@@ -7351,8 +7363,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A206" s="27">
+    <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206">
         <v>16</v>
       </c>
       <c r="B206" s="15" t="s">
@@ -7374,67 +7386,64 @@
         <v>50</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A207" s="27">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207">
         <v>17</v>
       </c>
-      <c r="B207" s="15" t="s">
+      <c r="B207" t="s">
         <v>527</v>
       </c>
-      <c r="C207" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D207" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E207" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="F207" s="15">
+      <c r="C207" t="s">
+        <v>572</v>
+      </c>
+      <c r="D207" t="s">
+        <v>573</v>
+      </c>
+      <c r="E207" t="s">
+        <v>544</v>
+      </c>
+      <c r="F207">
         <v>8</v>
       </c>
       <c r="I207" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A208" s="27">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208">
         <v>18</v>
       </c>
-      <c r="B208" s="15" t="s">
+      <c r="B208" t="s">
         <v>527</v>
       </c>
-      <c r="C208" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D208" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E208" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F208" s="15">
-        <v>1</v>
+      <c r="C208" t="s">
+        <v>574</v>
+      </c>
+      <c r="D208" t="s">
+        <v>575</v>
+      </c>
+      <c r="E208" t="s">
+        <v>544</v>
+      </c>
+      <c r="F208">
+        <v>8</v>
       </c>
       <c r="I208" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J208" s="15" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A209" s="27">
+      <c r="A209">
         <v>19</v>
       </c>
       <c r="B209" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C209" s="15" t="s">
-        <v>480</v>
+        <v>65</v>
       </c>
       <c r="D209" s="15" t="s">
-        <v>481</v>
+        <v>98</v>
       </c>
       <c r="E209" s="15" t="s">
         <v>528</v>
@@ -7445,48 +7454,45 @@
       <c r="I209" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J209" s="15" t="s">
-        <v>480</v>
-      </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A210" s="27">
+      <c r="A210">
         <v>20</v>
       </c>
       <c r="B210" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C210" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D210" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E210" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F210" s="15">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="I210" s="15" t="s">
         <v>50</v>
       </c>
       <c r="J210" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A211" s="27">
+      <c r="A211">
         <v>21</v>
       </c>
       <c r="B211" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C211" s="15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D211" s="15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E211" s="15" t="s">
         <v>528</v>
@@ -7498,21 +7504,21 @@
         <v>50</v>
       </c>
       <c r="J211" s="15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A212" s="27">
+      <c r="A212">
         <v>22</v>
       </c>
       <c r="B212" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C212" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D212" s="15" t="s">
-        <v>531</v>
+        <v>101</v>
       </c>
       <c r="E212" s="15" t="s">
         <v>108</v>
@@ -7524,21 +7530,21 @@
         <v>50</v>
       </c>
       <c r="J212" s="15" t="s">
-        <v>484</v>
+        <v>68</v>
       </c>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A213" s="27">
-        <v>25</v>
+      <c r="A213">
+        <v>23</v>
       </c>
       <c r="B213" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C213" s="15" t="s">
-        <v>532</v>
+        <v>482</v>
       </c>
       <c r="D213" s="15" t="s">
-        <v>533</v>
+        <v>483</v>
       </c>
       <c r="E213" s="15" t="s">
         <v>528</v>
@@ -7549,74 +7555,74 @@
       <c r="I213" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J213" t="s">
-        <v>486</v>
+      <c r="J213" s="15" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A214" s="27">
-        <v>26</v>
+      <c r="A214">
+        <v>24</v>
       </c>
       <c r="B214" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C214" s="15" t="s">
-        <v>468</v>
+        <v>69</v>
       </c>
       <c r="D214" s="15" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E214" s="15" t="s">
-        <v>528</v>
+        <v>108</v>
       </c>
       <c r="F214" s="15">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I214" s="15" t="s">
         <v>50</v>
       </c>
       <c r="J214" s="15" t="s">
-        <v>468</v>
+        <v>484</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A215" s="27">
-        <v>27</v>
+      <c r="A215">
+        <v>25</v>
       </c>
       <c r="B215" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C215" s="15" t="s">
-        <v>470</v>
+        <v>532</v>
       </c>
       <c r="D215" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E215" s="15" t="s">
-        <v>108</v>
+        <v>528</v>
       </c>
       <c r="F215" s="15">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I215" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J215" s="15" t="s">
-        <v>470</v>
+      <c r="J215" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A216" s="27">
-        <v>28</v>
+      <c r="A216">
+        <v>26</v>
       </c>
       <c r="B216" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C216" s="15" t="s">
-        <v>518</v>
+        <v>468</v>
       </c>
       <c r="D216" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E216" s="15" t="s">
         <v>528</v>
@@ -7628,70 +7634,73 @@
         <v>50</v>
       </c>
       <c r="J216" s="15" t="s">
-        <v>518</v>
+        <v>468</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A217" s="27">
-        <v>29</v>
+      <c r="A217">
+        <v>27</v>
       </c>
       <c r="B217" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C217" s="15" t="s">
-        <v>537</v>
+        <v>470</v>
       </c>
       <c r="D217" s="15" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E217" s="15" t="s">
-        <v>528</v>
+        <v>108</v>
       </c>
       <c r="F217" s="15">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I217" s="15" t="s">
         <v>50</v>
       </c>
       <c r="J217" s="15" t="s">
-        <v>518</v>
+        <v>470</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A218" s="27">
-        <v>30</v>
+      <c r="A218">
+        <v>28</v>
       </c>
       <c r="B218" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C218" s="15" t="s">
-        <v>465</v>
+        <v>518</v>
       </c>
       <c r="D218" s="15" t="s">
-        <v>86</v>
+        <v>536</v>
       </c>
       <c r="E218" s="15" t="s">
-        <v>108</v>
+        <v>528</v>
       </c>
       <c r="F218" s="15">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I218" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="27">
-        <v>31</v>
+      <c r="J218" s="15" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>29</v>
       </c>
       <c r="B219" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C219" s="15" t="s">
-        <v>466</v>
+        <v>537</v>
       </c>
       <c r="D219" s="15" t="s">
-        <v>467</v>
+        <v>538</v>
       </c>
       <c r="E219" s="15" t="s">
         <v>528</v>
@@ -7703,21 +7712,21 @@
         <v>50</v>
       </c>
       <c r="J219" s="15" t="s">
-        <v>466</v>
+        <v>518</v>
       </c>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A220" s="27">
-        <v>32</v>
+      <c r="A220">
+        <v>30</v>
       </c>
       <c r="B220" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C220" s="15" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D220" s="15" t="s">
-        <v>539</v>
+        <v>86</v>
       </c>
       <c r="E220" s="15" t="s">
         <v>108</v>
@@ -7729,18 +7738,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A221" s="27">
-        <v>33</v>
+    <row r="221" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>31</v>
       </c>
       <c r="B221" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C221" s="15" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D221" s="15" t="s">
-        <v>540</v>
+        <v>467</v>
       </c>
       <c r="E221" s="15" t="s">
         <v>528</v>
@@ -7752,47 +7761,44 @@
         <v>50</v>
       </c>
       <c r="J221" s="15" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A222" s="27">
-        <v>36</v>
+      <c r="A222">
+        <v>32</v>
       </c>
       <c r="B222" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C222" s="15" t="s">
-        <v>74</v>
+        <v>461</v>
       </c>
       <c r="D222" s="15" t="s">
-        <v>106</v>
+        <v>539</v>
       </c>
       <c r="E222" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F222" s="15">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="I222" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J222" s="15" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A223" s="27">
-        <v>37</v>
+      <c r="A223">
+        <v>33</v>
       </c>
       <c r="B223" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C223" s="15" t="s">
-        <v>492</v>
+        <v>463</v>
       </c>
       <c r="D223" s="15" t="s">
-        <v>493</v>
+        <v>540</v>
       </c>
       <c r="E223" s="15" t="s">
         <v>528</v>
@@ -7804,50 +7810,50 @@
         <v>50</v>
       </c>
       <c r="J223" s="15" t="s">
-        <v>492</v>
+        <v>463</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A224" s="27">
-        <v>40</v>
+      <c r="A224">
+        <v>34</v>
       </c>
       <c r="B224" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C224" s="15" t="s">
-        <v>490</v>
+        <v>74</v>
       </c>
       <c r="D224" s="15" t="s">
-        <v>541</v>
+        <v>106</v>
       </c>
       <c r="E224" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F224" s="15">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="I224" s="15" t="s">
         <v>50</v>
       </c>
       <c r="J224" s="15" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A225" s="27">
-        <v>41</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>35</v>
       </c>
       <c r="B225" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C225" s="15" t="s">
-        <v>372</v>
+        <v>492</v>
       </c>
       <c r="D225" s="15" t="s">
-        <v>560</v>
+        <v>493</v>
       </c>
       <c r="E225" s="15" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="F225" s="15">
         <v>8</v>
@@ -7855,42 +7861,48 @@
       <c r="I225" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A226" s="27">
-        <v>45</v>
+      <c r="J225" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>36</v>
       </c>
       <c r="B226" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C226" s="15" t="s">
-        <v>374</v>
+        <v>490</v>
       </c>
       <c r="D226" s="15" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
       <c r="E226" s="15" t="s">
-        <v>544</v>
+        <v>108</v>
       </c>
       <c r="F226" s="15">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I226" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A227" s="27">
-        <v>46</v>
+      <c r="J226" s="15" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>37</v>
       </c>
       <c r="B227" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C227" s="15" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D227" s="15" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E227" s="15" t="s">
         <v>544</v>
@@ -7902,18 +7914,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A228" s="27">
-        <v>47</v>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>38</v>
       </c>
       <c r="B228" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C228" s="15" t="s">
-        <v>477</v>
+        <v>374</v>
       </c>
       <c r="D228" s="15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E228" s="15" t="s">
         <v>544</v>
@@ -7925,18 +7937,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="27">
-        <v>48</v>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>39</v>
       </c>
       <c r="B229" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C229" s="15" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
       <c r="D229" s="15" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E229" s="15" t="s">
         <v>544</v>
@@ -7948,18 +7960,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A230" s="27">
-        <v>49</v>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>40</v>
       </c>
       <c r="B230" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C230" s="15" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="D230" s="15" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E230" s="15" t="s">
         <v>544</v>
@@ -7971,18 +7983,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A231" s="27">
-        <v>50</v>
+    <row r="231" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>41</v>
       </c>
       <c r="B231" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C231" s="15" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D231" s="15" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="E231" s="15" t="s">
         <v>544</v>
@@ -7994,18 +8006,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A232" s="27">
-        <v>51</v>
+    <row r="232" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>42</v>
       </c>
       <c r="B232" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C232" s="15" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="D232" s="15" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E232" s="15" t="s">
         <v>544</v>
@@ -8017,18 +8029,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A233" s="27">
-        <v>54</v>
+    <row r="233" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>43</v>
       </c>
       <c r="B233" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C233" s="15" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D233" s="15" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E233" s="15" t="s">
         <v>544</v>
@@ -8040,18 +8052,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A234" s="27">
-        <v>55</v>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>44</v>
       </c>
       <c r="B234" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C234" s="15" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D234" s="15" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E234" s="15" t="s">
         <v>544</v>
@@ -8063,21 +8075,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A235" s="27">
-        <v>56</v>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>45</v>
       </c>
       <c r="B235" s="15" t="s">
         <v>527</v>
       </c>
       <c r="C235" s="15" t="s">
-        <v>384</v>
+        <v>502</v>
       </c>
       <c r="D235" s="15" t="s">
-        <v>385</v>
+        <v>568</v>
       </c>
       <c r="E235" s="15" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="F235" s="15">
         <v>8</v>
@@ -8086,44 +8098,84 @@
         <v>50</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A236" s="27"/>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A237" s="27"/>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A238" s="27"/>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A239" s="27"/>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A240" s="27"/>
+    <row r="236" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>46</v>
+      </c>
+      <c r="B236" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="C236" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="D236" s="15" t="s">
+        <v>569</v>
+      </c>
+      <c r="E236" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="F236" s="15">
+        <v>8</v>
+      </c>
+      <c r="I236" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>47</v>
+      </c>
+      <c r="B237" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="C237" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D237" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="E237" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="F237" s="15">
+        <v>8</v>
+      </c>
+      <c r="I237" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A238"/>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A239"/>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A240"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="27"/>
+      <c r="A241"/>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="27"/>
+      <c r="A242"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="27"/>
+      <c r="A243"/>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="27"/>
+      <c r="A244"/>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="27"/>
+      <c r="A245"/>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="27"/>
+      <c r="A246"/>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="27"/>
+      <c r="A247"/>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="27"/>
+      <c r="A248"/>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="27"/>
@@ -8152,8 +8204,14 @@
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="27"/>
     </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="27"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="27"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P235" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:P237" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>